<commit_message>
beresin dashboard, sisa filterig prodi
</commit_message>
<xml_diff>
--- a/public/sheets/ex-jadwal.xlsx
+++ b/public/sheets/ex-jadwal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25ACD6F-A3BE-4B0C-BC69-91204029DFB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1659BD9-27D1-4C7B-AA53-A9BBFB55BD2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{6827552D-A082-4B33-8C73-6D59A9B0D37E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{6827552D-A082-4B33-8C73-6D59A9B0D37E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -67,7 +67,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -92,13 +92,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -113,8 +113,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="1457325"/>
-          <a:ext cx="6286500" cy="809624"/>
+          <a:off x="0" y="1333500"/>
+          <a:ext cx="7172324" cy="809624"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -168,18 +168,18 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>row[0]   |  row[1]   |   row[2]   |  row[3]   |  row[4]   |   row[5]   |  row[6]   |  row[7]   |  row[8]   |   row[9]   |</a:t>
+            <a:t>row[0]   | row[1]   |  row[2]   |   row[3]   |  row[4]   |  row[5]   |   row[6]   |  row[7]   |  row[8]   |  row[9]        |   row[10]   |</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>kelas_id| matkul_id| dosen_id|</a:t>
+            <a:t>prodi_id | kelas_id| matkul_id| dosen_id|</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> ruang_id|semester| sks           | jml_jam | hr (hari) | jam_awal|jam_akhir|</a:t>
+            <a:t> ruang_id|semester| sks           | jml_jam | hr (hari) | jam_awal    |jam_akhir|</a:t>
           </a:r>
           <a:endParaRPr lang="id-ID" sz="1100"/>
         </a:p>
@@ -487,255 +487,276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C449466-A3B0-4804-B9FB-8AB829C689B6}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
         <v>17</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>16</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>6</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>3</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>4</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>1</v>
       </c>
-      <c r="I1" s="2">
+      <c r="J1" s="2">
         <v>0.3611111111111111</v>
       </c>
-      <c r="J1" s="2">
+      <c r="K1" s="2">
         <v>0.5</v>
       </c>
-      <c r="K1" s="1"/>
       <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>25</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>14</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>6</v>
       </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
       <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
         <v>3</v>
       </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>0.64583333333333337</v>
       </c>
-      <c r="K2" s="1"/>
       <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>22</v>
       </c>
-      <c r="D3">
-        <v>11</v>
-      </c>
       <c r="E3">
+        <v>11</v>
+      </c>
+      <c r="F3">
         <v>6</v>
       </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
       <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
         <v>3</v>
       </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3" s="2">
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2">
         <v>0.39583333333333331</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>0.5</v>
       </c>
-      <c r="K3" s="1"/>
       <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
+        <v>11</v>
+      </c>
+      <c r="C4">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>22</v>
       </c>
-      <c r="D4">
-        <v>11</v>
-      </c>
       <c r="E4">
+        <v>11</v>
+      </c>
+      <c r="F4">
         <v>6</v>
       </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4">
         <v>2</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2">
         <v>0.61111111111111105</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>0.68055555555555547</v>
       </c>
-      <c r="K4" s="1"/>
       <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>18</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>16</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>6</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>4</v>
       </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2">
         <v>0.68055555555555547</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>0.84027777777777779</v>
       </c>
-      <c r="K5" s="1"/>
       <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>23</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>10</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>6</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>3</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>5</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>4</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>0.3611111111111111</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>0.5</v>
       </c>
-      <c r="K6" s="1"/>
       <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="C7">
         <v>7</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>19</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>16</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>6</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>3</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
       </c>
       <c r="H7">
         <v>4</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7" s="2">
         <v>0.68055555555555547</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>0.84027777777777779</v>
       </c>
-      <c r="K7" s="1"/>
       <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>